<commit_message>
parseRecipe root will now return a parsed recipe
</commit_message>
<xml_diff>
--- a/tools/excel/Misc.xlsx
+++ b/tools/excel/Misc.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Kutenq-backend\tools\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D1042A-A73A-408A-829A-64AD2F4D437A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B8EBA6-3AE2-4ADB-8114-57C19E1E8B3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D33C6BDB-7E0B-4C3C-87D8-7817E9CC9260}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D33C6BDB-7E0B-4C3C-87D8-7817E9CC9260}"/>
   </bookViews>
   <sheets>
     <sheet name="dotenvs" sheetId="1" r:id="rId1"/>
     <sheet name="routes" sheetId="2" r:id="rId2"/>
+    <sheet name="localizedRegex" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="51">
   <si>
     <t>Name</t>
   </si>
@@ -116,6 +117,9 @@
     <t>Logs any file-system related inquiries</t>
   </si>
   <si>
+    <t>Type</t>
+  </si>
+  <si>
     <t>GET</t>
   </si>
   <si>
@@ -126,13 +130,275 @@
   </si>
   <si>
     <t>type, data*</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>mongo_host</t>
+  </si>
+  <si>
+    <t>MongoDB host</t>
+  </si>
+  <si>
+    <t>mongodb://localhost:27017</t>
+  </si>
+  <si>
+    <t>mongo_database</t>
+  </si>
+  <si>
+    <t>MongoDB database</t>
+  </si>
+  <si>
+    <t>kutenq</t>
+  </si>
+  <si>
+    <t>Locale</t>
+  </si>
+  <si>
+    <t>en</t>
+  </si>
+  <si>
+    <t>Reigon</t>
+  </si>
+  <si>
+    <t>aOfRegex</t>
+  </si>
+  <si>
+    <t>regex</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <r>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC678DD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>^</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF56B6C2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(?:"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD19A66"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF56B6C2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD19A66"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF56B6C2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD19A66"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF56B6C2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)(?:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF56B6C2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>of)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF98C379"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC678DD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>i</t>
+    </r>
+  </si>
+  <si>
+    <t>Regex for testing food. Tests "A ### of" and captures ###</t>
+  </si>
+  <si>
+    <t>noteRegex</t>
+  </si>
+  <si>
+    <r>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF56B6C2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(?:\()(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD19A66"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF56B6C2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)(?:\))</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFABB2BF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF56B6C2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE06C75"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF98C379"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>/</t>
+    </r>
+  </si>
+  <si>
+    <t>Recipe Parsing</t>
+  </si>
+  <si>
+    <t>Regex for capturing notes. Tests (###) or ;###</t>
+  </si>
+  <si>
+    <t>Localized Regex</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,6 +413,47 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFABB2BF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF98C379"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC678DD"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF56B6C2"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFD19A66"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFE06C75"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -179,7 +486,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -191,16 +498,107 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
+  <dxfs count="23">
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF98C379"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thick">
+          <color theme="4"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -228,10 +626,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -257,11 +651,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4094A646-40A1-4EE1-A544-7AAC009FEEE5}" name="Table1" displayName="Table1" ref="A2:D6" totalsRowShown="0" dataDxfId="13">
-  <autoFilter ref="A2:D6" xr:uid="{4094A646-40A1-4EE1-A544-7AAC009FEEE5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4094A646-40A1-4EE1-A544-7AAC009FEEE5}" name="Table1" displayName="Table1" ref="A2:D8" totalsRowShown="0" dataDxfId="22">
+  <autoFilter ref="A2:D8" xr:uid="{4094A646-40A1-4EE1-A544-7AAC009FEEE5}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{33E47659-9318-42EC-A492-63F14C707FD1}" name="Category" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{719B405F-41E2-4908-A2F1-D2E11D989824}" name="Name" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{33E47659-9318-42EC-A492-63F14C707FD1}" name="Category" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{719B405F-41E2-4908-A2F1-D2E11D989824}" name="Name" dataDxfId="20"/>
     <tableColumn id="3" xr3:uid="{5939A71D-FA98-4D3F-AB17-C57E90E880C1}" name="Description" dataDxfId="10"/>
     <tableColumn id="4" xr3:uid="{109998A6-10DB-4C05-A72D-1E4599CB51FF}" name="Default Value" dataDxfId="9"/>
   </tableColumns>
@@ -270,16 +664,32 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B6268529-956C-4A56-BD27-1FF0230454CD}" name="Table4" displayName="Table4" ref="A2:G4" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B6268529-956C-4A56-BD27-1FF0230454CD}" name="Table4" displayName="Table4" ref="A2:G4" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="A2:G4" xr:uid="{B6268529-956C-4A56-BD27-1FF0230454CD}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{4A43527B-A0C6-4EB7-85FE-0D3AE91B1CAC}" name="Controller" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{5225B744-39FC-46D7-819C-E8E60D34E917}" name="Name" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{89B3C17C-2256-4B80-9D94-B0A92E527C66}" name="Function" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{5B9B5968-26EA-4FE4-96D0-43821F04CC59}" name="Params" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{E161B320-73DB-4C75-A3B9-B9B4FE1DA924}" name="Function req args" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{99003681-E7C8-4383-BBFB-3BD00919E8EC}" name="Description" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{13E1FCD1-7463-4C8C-AA21-9D582F5E6FCF}" name="Method" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{4A43527B-A0C6-4EB7-85FE-0D3AE91B1CAC}" name="Controller" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{5225B744-39FC-46D7-819C-E8E60D34E917}" name="Name" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{89B3C17C-2256-4B80-9D94-B0A92E527C66}" name="Function" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{5B9B5968-26EA-4FE4-96D0-43821F04CC59}" name="Params" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{E161B320-73DB-4C75-A3B9-B9B4FE1DA924}" name="Function req args" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{99003681-E7C8-4383-BBFB-3BD00919E8EC}" name="Description" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{13E1FCD1-7463-4C8C-AA21-9D582F5E6FCF}" name="Method" dataDxfId="11"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2604A3C4-082F-46B4-B43F-397841C4F5F4}" name="Table2" displayName="Table2" ref="A2:G4" totalsRowShown="0" dataDxfId="6" tableBorderDxfId="8">
+  <autoFilter ref="A2:G4" xr:uid="{2604A3C4-082F-46B4-B43F-397841C4F5F4}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{BC9D71B9-C890-43E6-9A1A-44FD8BD40DF5}" name="Locale" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{B9420AE5-ECA9-423F-B897-15287A427AB7}" name="Reigon" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{D14B1528-68B5-46CA-BF93-5BE266A33E88}" name="Category" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{9D26CB89-5F50-42A6-9BA3-EE03A85CBE10}" name="Name" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{5C23A4CA-234A-48AF-ABDC-96D684FB0A38}" name="Value" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{463ED3D5-F4C3-4A5E-9A4E-53AC750E36F9}" name="Type" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{E09F8376-4004-4503-B1CD-07E9B2A6C180}" name="Description" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -582,10 +992,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33D156AB-8D24-4FA1-88BF-664050F6EF77}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="D2" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,7 +1003,7 @@
     <col min="1" max="1" width="14.140625" customWidth="1"/>
     <col min="2" max="2" width="21.140625" customWidth="1"/>
     <col min="3" max="3" width="61.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -614,7 +1024,7 @@
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
     </row>
@@ -628,7 +1038,7 @@
       <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="2" t="b">
+      <c r="D3" s="7" t="b">
         <v>1</v>
       </c>
     </row>
@@ -642,7 +1052,7 @@
       <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="2" t="b">
+      <c r="D4" s="7" t="b">
         <v>0</v>
       </c>
     </row>
@@ -656,7 +1066,7 @@
       <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="2" t="b">
+      <c r="D5" s="7" t="b">
         <v>0</v>
       </c>
     </row>
@@ -670,8 +1080,36 @@
       <c r="C6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="2" t="b">
+      <c r="D6" s="7" t="b">
         <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -689,7 +1127,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ABD49B9-4C0C-4D6E-9938-2A8DD210C020}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -705,15 +1143,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -735,7 +1173,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -749,14 +1187,14 @@
         <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -770,14 +1208,14 @@
         <v>16</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
         <v>23</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -789,4 +1227,111 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7370F629-F629-4A97-B97F-8F39179752CB}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="67.42578125" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Route to get LDJSON, added more fields
</commit_message>
<xml_diff>
--- a/tools/excel/Misc.xlsx
+++ b/tools/excel/Misc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Kutenq-backend\tools\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B8EBA6-3AE2-4ADB-8114-57C19E1E8B3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7FB606D-1C84-4357-92D8-69ABD7E5C010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D33C6BDB-7E0B-4C3C-87D8-7817E9CC9260}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D33C6BDB-7E0B-4C3C-87D8-7817E9CC9260}"/>
   </bookViews>
   <sheets>
     <sheet name="dotenvs" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="55">
   <si>
     <t>Name</t>
   </si>
@@ -392,6 +392,18 @@
   </si>
   <si>
     <t>Localized Regex</t>
+  </si>
+  <si>
+    <t>url*</t>
+  </si>
+  <si>
+    <t>getLDJSONfromURL</t>
+  </si>
+  <si>
+    <t>Gets LD JSON from a url</t>
+  </si>
+  <si>
+    <t>Gets LD JSON</t>
   </si>
 </sst>
 </file>
@@ -664,8 +676,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B6268529-956C-4A56-BD27-1FF0230454CD}" name="Table4" displayName="Table4" ref="A2:G4" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
-  <autoFilter ref="A2:G4" xr:uid="{B6268529-956C-4A56-BD27-1FF0230454CD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B6268529-956C-4A56-BD27-1FF0230454CD}" name="Table4" displayName="Table4" ref="A2:G5" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="A2:G5" xr:uid="{B6268529-956C-4A56-BD27-1FF0230454CD}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{4A43527B-A0C6-4EB7-85FE-0D3AE91B1CAC}" name="Controller" dataDxfId="17"/>
     <tableColumn id="2" xr3:uid="{5225B744-39FC-46D7-819C-E8E60D34E917}" name="Name" dataDxfId="16"/>
@@ -1125,17 +1137,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ABD49B9-4C0C-4D6E-9938-2A8DD210C020}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
     <col min="5" max="5" width="23.28515625" customWidth="1"/>
     <col min="6" max="6" width="33.5703125" customWidth="1"/>
@@ -1217,6 +1229,25 @@
       <c r="G4" s="2" t="s">
         <v>27</v>
       </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1233,8 +1264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7370F629-F629-4A97-B97F-8F39179752CB}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Merged frontend and backend into one git repo
</commit_message>
<xml_diff>
--- a/tools/excel/Misc.xlsx
+++ b/tools/excel/Misc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Kutenq-backend\tools\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F45A1049-F61B-4AC4-90F4-83C1B08B7815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A77E28-19CF-4BD0-88AA-8B0157415DE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D33C6BDB-7E0B-4C3C-87D8-7817E9CC9260}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D33C6BDB-7E0B-4C3C-87D8-7817E9CC9260}"/>
   </bookViews>
   <sheets>
     <sheet name="dotenvs" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="69">
   <si>
     <t>Name</t>
   </si>
@@ -428,6 +428,24 @@
   </si>
   <si>
     <t>Registers a user</t>
+  </si>
+  <si>
+    <t>locale</t>
+  </si>
+  <si>
+    <t>Get Locale</t>
+  </si>
+  <si>
+    <t>getLocale</t>
+  </si>
+  <si>
+    <t>Gets a locale file. Returns 'en' if none specified</t>
+  </si>
+  <si>
+    <t>default_locale</t>
+  </si>
+  <si>
+    <t>The default locale for kutenq!</t>
   </si>
 </sst>
 </file>
@@ -531,14 +549,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -549,9 +561,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -561,6 +570,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -568,40 +586,10 @@
   </cellStyles>
   <dxfs count="23">
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -642,7 +630,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -656,6 +644,36 @@
           <color theme="4"/>
         </top>
       </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -687,8 +705,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4094A646-40A1-4EE1-A544-7AAC009FEEE5}" name="Table1" displayName="Table1" ref="A2:D8" totalsRowShown="0" dataDxfId="22">
-  <autoFilter ref="A2:D8" xr:uid="{4094A646-40A1-4EE1-A544-7AAC009FEEE5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4094A646-40A1-4EE1-A544-7AAC009FEEE5}" name="Table1" displayName="Table1" ref="A2:D9" totalsRowShown="0" dataDxfId="22">
+  <autoFilter ref="A2:D9" xr:uid="{4094A646-40A1-4EE1-A544-7AAC009FEEE5}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{33E47659-9318-42EC-A492-63F14C707FD1}" name="Category" dataDxfId="21"/>
     <tableColumn id="2" xr3:uid="{719B405F-41E2-4908-A2F1-D2E11D989824}" name="Name" dataDxfId="20"/>
@@ -700,32 +718,32 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B6268529-956C-4A56-BD27-1FF0230454CD}" name="Table4" displayName="Table4" ref="A2:G7" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A2:G7" xr:uid="{B6268529-956C-4A56-BD27-1FF0230454CD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B6268529-956C-4A56-BD27-1FF0230454CD}" name="Table4" displayName="Table4" ref="A2:G8" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="A2:G8" xr:uid="{B6268529-956C-4A56-BD27-1FF0230454CD}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{4A43527B-A0C6-4EB7-85FE-0D3AE91B1CAC}" name="Controller" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{5225B744-39FC-46D7-819C-E8E60D34E917}" name="Name" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{89B3C17C-2256-4B80-9D94-B0A92E527C66}" name="Function" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{5B9B5968-26EA-4FE4-96D0-43821F04CC59}" name="Params" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{E161B320-73DB-4C75-A3B9-B9B4FE1DA924}" name="Function req args" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{99003681-E7C8-4383-BBFB-3BD00919E8EC}" name="Description" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{13E1FCD1-7463-4C8C-AA21-9D582F5E6FCF}" name="Method" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{4A43527B-A0C6-4EB7-85FE-0D3AE91B1CAC}" name="Controller" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{5225B744-39FC-46D7-819C-E8E60D34E917}" name="Name" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{89B3C17C-2256-4B80-9D94-B0A92E527C66}" name="Function" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{5B9B5968-26EA-4FE4-96D0-43821F04CC59}" name="Params" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{E161B320-73DB-4C75-A3B9-B9B4FE1DA924}" name="Function req args" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{99003681-E7C8-4383-BBFB-3BD00919E8EC}" name="Description" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{13E1FCD1-7463-4C8C-AA21-9D582F5E6FCF}" name="Method" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2604A3C4-082F-46B4-B43F-397841C4F5F4}" name="Table2" displayName="Table2" ref="A2:G4" totalsRowShown="0" dataDxfId="15" tableBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2604A3C4-082F-46B4-B43F-397841C4F5F4}" name="Table2" displayName="Table2" ref="A2:G4" totalsRowShown="0" dataDxfId="8" tableBorderDxfId="7">
   <autoFilter ref="A2:G4" xr:uid="{2604A3C4-082F-46B4-B43F-397841C4F5F4}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{BC9D71B9-C890-43E6-9A1A-44FD8BD40DF5}" name="Locale" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{B9420AE5-ECA9-423F-B897-15287A427AB7}" name="Reigon" dataDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{D14B1528-68B5-46CA-BF93-5BE266A33E88}" name="Category" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{9D26CB89-5F50-42A6-9BA3-EE03A85CBE10}" name="Name" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{5C23A4CA-234A-48AF-ABDC-96D684FB0A38}" name="Value" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{463ED3D5-F4C3-4A5E-9A4E-53AC750E36F9}" name="Type" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{E09F8376-4004-4503-B1CD-07E9B2A6C180}" name="Description" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{BC9D71B9-C890-43E6-9A1A-44FD8BD40DF5}" name="Locale" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{B9420AE5-ECA9-423F-B897-15287A427AB7}" name="Reigon" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{D14B1528-68B5-46CA-BF93-5BE266A33E88}" name="Category" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{9D26CB89-5F50-42A6-9BA3-EE03A85CBE10}" name="Name" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{5C23A4CA-234A-48AF-ABDC-96D684FB0A38}" name="Value" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{463ED3D5-F4C3-4A5E-9A4E-53AC750E36F9}" name="Type" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{E09F8376-4004-4503-B1CD-07E9B2A6C180}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1028,10 +1046,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33D156AB-8D24-4FA1-88BF-664050F6EF77}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1039,16 +1057,16 @@
     <col min="1" max="1" width="14.140625" customWidth="1"/>
     <col min="2" max="2" width="21.140625" customWidth="1"/>
     <col min="3" max="3" width="61.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1060,7 +1078,7 @@
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1074,7 +1092,7 @@
       <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="7" t="b">
+      <c r="D3" s="5" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1088,7 +1106,7 @@
       <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="7" t="b">
+      <c r="D4" s="5" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1102,7 +1120,7 @@
       <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="7" t="b">
+      <c r="D5" s="5" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1116,7 +1134,7 @@
       <c r="C6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="7" t="b">
+      <c r="D6" s="5" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1130,7 +1148,7 @@
       <c r="C7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="5" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1144,8 +1162,22 @@
       <c r="C8" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="5" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1161,10 +1193,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ABD49B9-4C0C-4D6E-9938-2A8DD210C020}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1179,15 +1211,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1311,6 +1343,27 @@
       </c>
       <c r="G7" s="2" t="s">
         <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1344,15 +1397,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1378,44 +1431,44 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8" t="s">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="8" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8" t="s">
+      <c r="B4" s="6"/>
+      <c r="C4" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="8" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Database stuffs, getting locales
</commit_message>
<xml_diff>
--- a/tools/excel/Misc.xlsx
+++ b/tools/excel/Misc.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Kutenq-backend\tools\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\kutenq\tools\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A77E28-19CF-4BD0-88AA-8B0157415DE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77BAB88F-7247-4299-83AA-3E2D1BA166CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D33C6BDB-7E0B-4C3C-87D8-7817E9CC9260}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="74">
   <si>
     <t>Name</t>
   </si>
@@ -446,6 +446,21 @@
   </si>
   <si>
     <t>The default locale for kutenq!</t>
+  </si>
+  <si>
+    <t>db_type</t>
+  </si>
+  <si>
+    <t>The type of database to use</t>
+  </si>
+  <si>
+    <t>mongodb</t>
+  </si>
+  <si>
+    <t>log_db</t>
+  </si>
+  <si>
+    <t>Log database</t>
   </si>
 </sst>
 </file>
@@ -705,8 +720,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4094A646-40A1-4EE1-A544-7AAC009FEEE5}" name="Table1" displayName="Table1" ref="A2:D9" totalsRowShown="0" dataDxfId="22">
-  <autoFilter ref="A2:D9" xr:uid="{4094A646-40A1-4EE1-A544-7AAC009FEEE5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4094A646-40A1-4EE1-A544-7AAC009FEEE5}" name="Table1" displayName="Table1" ref="A2:D11" totalsRowShown="0" dataDxfId="22">
+  <autoFilter ref="A2:D11" xr:uid="{4094A646-40A1-4EE1-A544-7AAC009FEEE5}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{33E47659-9318-42EC-A492-63F14C707FD1}" name="Category" dataDxfId="21"/>
     <tableColumn id="2" xr3:uid="{719B405F-41E2-4908-A2F1-D2E11D989824}" name="Name" dataDxfId="20"/>
@@ -1046,10 +1061,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33D156AB-8D24-4FA1-88BF-664050F6EF77}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1178,6 +1193,34 @@
       </c>
       <c r="D9" s="5" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="5" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>